<commit_message>
Updated metrics.xlsx for 2/9/12
</commit_message>
<xml_diff>
--- a/doc/metrics.xlsx
+++ b/doc/metrics.xlsx
@@ -123,10 +123,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$D$1</c:f>
+              <c:f>Sheet1!$B$1:$E$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -135,16 +135,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>40941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$D$2</c:f>
+              <c:f>Sheet1!$B$2:$E$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -152,6 +155,9 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
@@ -177,10 +183,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$D$1</c:f>
+              <c:f>Sheet1!$B$1:$E$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -189,16 +195,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>40941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$D$3</c:f>
+              <c:f>Sheet1!$B$3:$E$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -206,6 +215,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -231,10 +243,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$D$1</c:f>
+              <c:f>Sheet1!$B$1:$E$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -243,16 +255,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>40941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$D$4</c:f>
+              <c:f>Sheet1!$B$4:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>47</c:v>
                 </c:pt>
@@ -260,6 +275,9 @@
                   <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>47</c:v>
                 </c:pt>
               </c:numCache>
@@ -285,10 +303,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$D$1</c:f>
+              <c:f>Sheet1!$B$1:$E$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -297,16 +315,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>40941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$D$5</c:f>
+              <c:f>Sheet1!$B$5:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>70</c:v>
                 </c:pt>
@@ -321,18 +342,18 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="57835904"/>
-        <c:axId val="57837440"/>
+        <c:axId val="85979904"/>
+        <c:axId val="86254720"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="57835904"/>
+        <c:axId val="85979904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57837440"/>
+        <c:crossAx val="86254720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -340,7 +361,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="57837440"/>
+        <c:axId val="86254720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -348,7 +369,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57835904"/>
+        <c:crossAx val="85979904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -359,10 +380,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.66823091247672251"/>
-          <c:y val="4.3679125262180658E-2"/>
+          <c:x val="0.66823091247672273"/>
+          <c:y val="4.3679125262180644E-2"/>
           <c:w val="0.30569832402234637"/>
-          <c:h val="0.906819333172873"/>
+          <c:h val="0.90681933317287311"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -370,7 +391,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -403,10 +424,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$D$7</c:f>
+              <c:f>Sheet1!$B$7:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -415,18 +436,24 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>40941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$D$8</c:f>
+              <c:f>Sheet1!$B$8:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="2">
                   <c:v>8825</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9092</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -451,10 +478,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$D$7</c:f>
+              <c:f>Sheet1!$B$7:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -463,29 +490,35 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>40941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$D$9</c:f>
+              <c:f>Sheet1!$B$9:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="2">
                   <c:v>6499</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6693</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="92548480"/>
-        <c:axId val="92845568"/>
+        <c:axId val="91699456"/>
+        <c:axId val="91713536"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="92548480"/>
+        <c:axId val="91699456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -502,7 +535,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92845568"/>
+        <c:crossAx val="91713536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -511,7 +544,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="92845568"/>
+        <c:axId val="91713536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -519,7 +552,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92548480"/>
+        <c:crossAx val="91699456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -532,7 +565,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -568,10 +601,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$D$7</c:f>
+              <c:f>Sheet1!$B$7:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -580,16 +613,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>40941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$D$11</c:f>
+              <c:f>Sheet1!$B$11:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>85</c:v>
                 </c:pt>
@@ -598,24 +634,27 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="36892672"/>
-        <c:axId val="36894208"/>
+        <c:axId val="91727744"/>
+        <c:axId val="91729280"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="36892672"/>
+        <c:axId val="91727744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="36894208"/>
+        <c:crossAx val="91729280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -623,7 +662,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="36894208"/>
+        <c:axId val="91729280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -631,7 +670,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="36892672"/>
+        <c:crossAx val="91727744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -644,7 +683,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -677,10 +716,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$D$13</c:f>
+              <c:f>Sheet1!$B$13:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -689,16 +728,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>40941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$D$14</c:f>
+              <c:f>Sheet1!$B$14:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -706,6 +748,9 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
@@ -731,10 +776,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$D$13</c:f>
+              <c:f>Sheet1!$B$13:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -743,16 +788,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>40941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$D$15</c:f>
+              <c:f>Sheet1!$B$15:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -760,6 +808,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -785,10 +836,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$D$13</c:f>
+              <c:f>Sheet1!$B$13:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -797,16 +848,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>40941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$16:$D$16</c:f>
+              <c:f>Sheet1!$B$16:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -814,6 +868,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -839,10 +896,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$D$13</c:f>
+              <c:f>Sheet1!$B$13:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -851,16 +908,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>40941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$D$17</c:f>
+              <c:f>Sheet1!$B$17:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -868,6 +928,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -875,18 +938,18 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="99709312"/>
-        <c:axId val="99730560"/>
+        <c:axId val="90392448"/>
+        <c:axId val="90393984"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="99709312"/>
+        <c:axId val="90392448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99730560"/>
+        <c:crossAx val="90393984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -894,7 +957,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="99730560"/>
+        <c:axId val="90393984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -902,7 +965,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99709312"/>
+        <c:crossAx val="90392448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -913,7 +976,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.6966296296296296"/>
+          <c:x val="0.69662962962962971"/>
           <c:y val="6.1146374170477601E-2"/>
           <c:w val="0.28114814814814815"/>
           <c:h val="0.86898463019633465"/>
@@ -924,7 +987,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -964,16 +1027,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -994,16 +1057,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1340,10 +1403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1352,7 +1415,7 @@
     <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="B1" s="1">
         <v>40927</v>
       </c>
@@ -1362,8 +1425,11 @@
       <c r="D1" s="1">
         <v>40941</v>
       </c>
+      <c r="E1" s="1">
+        <v>40948</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1376,8 +1442,11 @@
       <c r="D2">
         <v>5</v>
       </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1390,8 +1459,11 @@
       <c r="D3">
         <v>0</v>
       </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1404,8 +1476,11 @@
       <c r="D4">
         <v>47</v>
       </c>
+      <c r="E4">
+        <v>47</v>
+      </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1419,7 +1494,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="B7" s="1">
         <v>40927</v>
       </c>
@@ -1429,24 +1504,33 @@
       <c r="D7" s="1">
         <v>40941</v>
       </c>
+      <c r="E7" s="1">
+        <v>40948</v>
+      </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="D8">
         <v>8825</v>
       </c>
+      <c r="E8">
+        <v>9092</v>
+      </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="D9">
         <v>6499</v>
       </c>
+      <c r="E9">
+        <v>6693</v>
+      </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1459,8 +1543,11 @@
       <c r="D11">
         <v>96</v>
       </c>
+      <c r="E11">
+        <v>97</v>
+      </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="B13" s="1">
         <v>40927</v>
       </c>
@@ -1470,8 +1557,11 @@
       <c r="D13" s="1">
         <v>40941</v>
       </c>
+      <c r="E13" s="1">
+        <v>40948</v>
+      </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1484,8 +1574,11 @@
       <c r="D14">
         <v>3</v>
       </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1498,8 +1591,11 @@
       <c r="D15">
         <v>1</v>
       </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1512,8 +1608,11 @@
       <c r="D16">
         <v>1</v>
       </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1524,6 +1623,9 @@
         <v>0</v>
       </c>
       <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added slides for today.
</commit_message>
<xml_diff>
--- a/doc/metrics.xlsx
+++ b/doc/metrics.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="14355" windowHeight="8760"/>
+    <workbookView xWindow="11980" yWindow="2100" windowWidth="24400" windowHeight="17600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -54,11 +59,27 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,14 +102,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -98,12 +131,24 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -123,46 +168,53 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$E$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>40927</c:v>
+              <c:f>Sheet1!$B$1:$F$1</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>40927.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40941</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40948</c:v>
+                  <c:v>40934.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40941.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40955.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$E$2</c:f>
+              <c:f>Sheet1!$B$2:$F$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -183,46 +235,53 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$E$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>40927</c:v>
+              <c:f>Sheet1!$B$1:$F$1</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>40927.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40941</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40948</c:v>
+                  <c:v>40934.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40941.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40955.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$E$3</c:f>
+              <c:f>Sheet1!$B$3:$F$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -243,46 +302,53 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$E$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>40927</c:v>
+              <c:f>Sheet1!$B$1:$F$1</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>40927.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40941</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40948</c:v>
+                  <c:v>40934.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40941.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40955.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$E$4</c:f>
+              <c:f>Sheet1!$B$4:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>47</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>47.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>47</c:v>
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -303,73 +369,99 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$E$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>40927</c:v>
+              <c:f>Sheet1!$B$1:$F$1</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>40927.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40941</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40948</c:v>
+                  <c:v>40934.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40941.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40955.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$E$5</c:f>
+              <c:f>Sheet1!$B$5:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>70</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>70.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>76</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>84</c:v>
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>93.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>101.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="85979904"/>
-        <c:axId val="86254720"/>
+        <c:smooth val="0"/>
+        <c:axId val="442512952"/>
+        <c:axId val="442516136"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="85979904"/>
+        <c:axId val="442512952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86254720"/>
+        <c:crossAx val="442516136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
-        <c:majorUnit val="7"/>
+        <c:baseTimeUnit val="days"/>
+        <c:majorUnit val="7.0"/>
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="86254720"/>
+        <c:axId val="442516136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85979904"/>
+        <c:crossAx val="442512952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -380,18 +472,21 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.66823091247672273"/>
-          <c:y val="4.3679125262180644E-2"/>
-          <c:w val="0.30569832402234637"/>
-          <c:h val="0.90681933317287311"/>
+          <c:x val="0.668230912476723"/>
+          <c:y val="0.0436791252621806"/>
+          <c:w val="0.305698324022346"/>
+          <c:h val="0.906819333172873"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -399,12 +494,24 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -424,40 +531,47 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$E$7</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>40927</c:v>
+              <c:f>Sheet1!$B$7:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>40927.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40941</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40948</c:v>
+                  <c:v>40934.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40941.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40955.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$E$8</c:f>
+              <c:f>Sheet1!$B$8:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="2">
-                  <c:v>8825</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9092</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="2">
+                  <c:v>8825.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9092.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9574.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -478,52 +592,71 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$E$7</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>40927</c:v>
+              <c:f>Sheet1!$B$7:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>40927.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40941</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40948</c:v>
+                  <c:v>40934.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40941.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40955.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$E$9</c:f>
+              <c:f>Sheet1!$B$9:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="2">
-                  <c:v>6499</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6693</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="2">
+                  <c:v>6499.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6693.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7025.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="91699456"/>
-        <c:axId val="91713536"/>
+        <c:smooth val="0"/>
+        <c:axId val="442574680"/>
+        <c:axId val="442577752"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="91699456"/>
+        <c:axId val="442574680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr rot="-2700000"/>
@@ -535,24 +668,27 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91713536"/>
+        <c:crossAx val="442577752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
-        <c:majorUnit val="7"/>
+        <c:majorUnit val="7.0"/>
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="91713536"/>
+        <c:axId val="442577752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91699456"/>
+        <c:crossAx val="442574680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -560,12 +696,15 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -573,15 +712,28 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -601,76 +753,100 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$E$7</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>40927</c:v>
+              <c:f>Sheet1!$B$7:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>40927.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40941</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40948</c:v>
+                  <c:v>40934.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40941.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40955.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$E$11</c:f>
+              <c:f>Sheet1!$B$11:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>85</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>85.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>97</c:v>
+                  <c:v>85.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>107.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="91727744"/>
-        <c:axId val="91729280"/>
+        <c:smooth val="0"/>
+        <c:axId val="442599544"/>
+        <c:axId val="442602568"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="91727744"/>
+        <c:axId val="442599544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91729280"/>
+        <c:crossAx val="442602568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
-        <c:majorUnit val="7"/>
+        <c:baseTimeUnit val="days"/>
+        <c:majorUnit val="7.0"/>
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="91729280"/>
+        <c:axId val="442602568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="80.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91727744"/>
+        <c:crossAx val="442599544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -678,12 +854,15 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -691,12 +870,24 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -716,46 +907,53 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$E$13</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>40927</c:v>
+              <c:f>Sheet1!$B$13:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>40927.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40941</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40948</c:v>
+                  <c:v>40934.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40941.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40955.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$E$14</c:f>
+              <c:f>Sheet1!$B$14:$F$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -776,46 +974,53 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$E$13</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>40927</c:v>
+              <c:f>Sheet1!$B$13:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>40927.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40941</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40948</c:v>
+                  <c:v>40934.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40941.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40955.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$E$15</c:f>
+              <c:f>Sheet1!$B$15:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -836,46 +1041,53 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$E$13</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>40927</c:v>
+              <c:f>Sheet1!$B$13:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>40927.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40941</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40948</c:v>
+                  <c:v>40934.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40941.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40955.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$16:$E$16</c:f>
+              <c:f>Sheet1!$B$16:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -896,76 +1108,99 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$E$13</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>40927</c:v>
+              <c:f>Sheet1!$B$13:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>40927.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40941</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40948</c:v>
+                  <c:v>40934.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40941.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40955.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$E$17</c:f>
+              <c:f>Sheet1!$B$17:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="90392448"/>
-        <c:axId val="90393984"/>
+        <c:smooth val="0"/>
+        <c:axId val="442646568"/>
+        <c:axId val="442649752"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="90392448"/>
+        <c:axId val="442646568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90393984"/>
+        <c:crossAx val="442649752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
-        <c:majorUnit val="7"/>
+        <c:baseTimeUnit val="days"/>
+        <c:majorUnit val="7.0"/>
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="90393984"/>
+        <c:axId val="442649752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90392448"/>
+        <c:crossAx val="442646568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -976,18 +1211,21 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.69662962962962971"/>
-          <c:y val="6.1146374170477601E-2"/>
-          <c:w val="0.28114814814814815"/>
-          <c:h val="0.86898463019633465"/>
+          <c:x val="0.69662962962963"/>
+          <c:y val="0.0611463741704776"/>
+          <c:w val="0.281148148148148"/>
+          <c:h val="0.868984630196335"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1402,20 +1640,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" s="1">
         <v>40927</v>
       </c>
@@ -1428,8 +1666,11 @@
       <c r="E1" s="1">
         <v>40948</v>
       </c>
+      <c r="F1" s="1">
+        <v>40955</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1445,8 +1686,11 @@
       <c r="E2">
         <v>5</v>
       </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1462,8 +1706,11 @@
       <c r="E3">
         <v>0</v>
       </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1479,8 +1726,11 @@
       <c r="E4">
         <v>47</v>
       </c>
+      <c r="F4">
+        <v>47</v>
+      </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1493,8 +1743,14 @@
       <c r="D5">
         <v>84</v>
       </c>
+      <c r="E5">
+        <v>93</v>
+      </c>
+      <c r="F5">
+        <v>101</v>
+      </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="B7" s="1">
         <v>40927</v>
       </c>
@@ -1507,8 +1763,11 @@
       <c r="E7" s="1">
         <v>40948</v>
       </c>
+      <c r="F7" s="1">
+        <v>40955</v>
+      </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1518,8 +1777,11 @@
       <c r="E8">
         <v>9092</v>
       </c>
+      <c r="F8">
+        <v>9574</v>
+      </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1529,8 +1791,11 @@
       <c r="E9">
         <v>6693</v>
       </c>
+      <c r="F9">
+        <v>7025</v>
+      </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1546,8 +1811,11 @@
       <c r="E11">
         <v>97</v>
       </c>
+      <c r="F11">
+        <v>107</v>
+      </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="B13" s="1">
         <v>40927</v>
       </c>
@@ -1560,8 +1828,11 @@
       <c r="E13" s="1">
         <v>40948</v>
       </c>
+      <c r="F13" s="1">
+        <v>40955</v>
+      </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1577,8 +1848,11 @@
       <c r="E14">
         <v>3</v>
       </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1594,8 +1868,11 @@
       <c r="E15">
         <v>1</v>
       </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1611,8 +1888,11 @@
       <c r="E16">
         <v>1</v>
       </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1626,36 +1906,54 @@
         <v>1</v>
       </c>
       <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added weekly status slides.  Updated metrics spreadsheet.  Deleted javadoc ant script since it doesn't use relative paths and I'm too lazy to fix that...
</commit_message>
<xml_diff>
--- a/doc/metrics.xlsx
+++ b/doc/metrics.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="2100" windowWidth="24400" windowHeight="17600"/>
+    <workbookView xWindow="11985" yWindow="2100" windowWidth="24405" windowHeight="17595"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,8 +59,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,24 +131,12 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -168,53 +156,58 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$F$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>40927.0</c:v>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>40927</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40941.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40948.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40955.0</c:v>
+                  <c:v>40934</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40955</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40962</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$F$2</c:f>
+              <c:f>Sheet1!$B$2:$G$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>116</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -235,53 +228,58 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$F$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>40927.0</c:v>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>40927</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40941.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40948.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40955.0</c:v>
+                  <c:v>40934</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40955</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40962</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$F$3</c:f>
+              <c:f>Sheet1!$B$3:$G$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -302,53 +300,58 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$F$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>40927.0</c:v>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>40927</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40941.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40948.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40955.0</c:v>
+                  <c:v>40934</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40955</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40962</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$F$4</c:f>
+              <c:f>Sheet1!$B$4:$G$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>47.0</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>47.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>47.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>47.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>47.0</c:v>
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>47</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -369,99 +372,90 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$F$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>40927.0</c:v>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>40927</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40941.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40948.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40955.0</c:v>
+                  <c:v>40934</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40955</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40962</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$F$5</c:f>
+              <c:f>Sheet1!$B$5:$G$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>70.0</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>76.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>84.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>93.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>101.0</c:v>
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>107</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="442512952"/>
-        <c:axId val="442516136"/>
+        <c:axId val="92125824"/>
+        <c:axId val="91427200"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="442512952"/>
+        <c:axId val="92125824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="442516136"/>
+        <c:crossAx val="91427200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
-        <c:majorUnit val="7.0"/>
+        <c:majorUnit val="7"/>
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="442516136"/>
+        <c:axId val="91427200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="442512952"/>
+        <c:crossAx val="92125824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -472,21 +466,19 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.668230912476723"/>
-          <c:y val="0.0436791252621806"/>
-          <c:w val="0.305698324022346"/>
-          <c:h val="0.906819333172873"/>
+          <c:x val="0.66823091247672317"/>
+          <c:y val="4.3679125262180617E-2"/>
+          <c:w val="0.30569832402234604"/>
+          <c:h val="0.90681933317287311"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -494,24 +486,12 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -531,47 +511,49 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$F$7</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>40927.0</c:v>
+              <c:f>Sheet1!$B$7:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>40927</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40941.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40948.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40955.0</c:v>
+                  <c:v>40934</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40955</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40962</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$F$8</c:f>
+              <c:f>Sheet1!$B$8:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="2">
-                  <c:v>8825.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9092.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9574.0</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="2">
+                  <c:v>8825</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9092</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9574</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -592,71 +574,62 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$F$7</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>40927.0</c:v>
+              <c:f>Sheet1!$B$7:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>40927</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40941.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40948.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40955.0</c:v>
+                  <c:v>40934</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40955</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40962</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$F$9</c:f>
+              <c:f>Sheet1!$B$9:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="2">
-                  <c:v>6499.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6693.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7025.0</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="2">
+                  <c:v>6499</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6693</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7025</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="442574680"/>
-        <c:axId val="442577752"/>
+        <c:axId val="91449600"/>
+        <c:axId val="91467776"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="442574680"/>
+        <c:axId val="91449600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr rot="-2700000"/>
@@ -668,27 +641,24 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442577752"/>
+        <c:crossAx val="91467776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
-        <c:majorUnit val="7.0"/>
+        <c:majorUnit val="7"/>
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="442577752"/>
+        <c:axId val="91467776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="442574680"/>
+        <c:crossAx val="91449600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -696,15 +666,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -712,28 +680,15 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -753,100 +708,88 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$F$7</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>40927.0</c:v>
+              <c:f>Sheet1!$B$7:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>40927</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40941.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40948.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40955.0</c:v>
+                  <c:v>40934</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40955</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40962</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$F$11</c:f>
+              <c:f>Sheet1!$B$11:$G$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>85.0</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>96.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>97.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>107.0</c:v>
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>107</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="442599544"/>
-        <c:axId val="442602568"/>
+        <c:axId val="92805376"/>
+        <c:axId val="92815360"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="442599544"/>
+        <c:axId val="92805376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="442602568"/>
+        <c:crossAx val="92815360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
-        <c:majorUnit val="7.0"/>
+        <c:majorUnit val="7"/>
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="442602568"/>
+        <c:axId val="92815360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="80.0"/>
+          <c:min val="80"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="442599544"/>
+        <c:crossAx val="92805376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -854,15 +797,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -870,24 +811,12 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -907,53 +836,58 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$F$13</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>40927.0</c:v>
+              <c:f>Sheet1!$B$13:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>40927</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40941.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40948.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40955.0</c:v>
+                  <c:v>40934</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40955</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40962</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$F$14</c:f>
+              <c:f>Sheet1!$B$14:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>3.0</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -974,53 +908,58 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$F$13</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>40927.0</c:v>
+              <c:f>Sheet1!$B$13:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>40927</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40941.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40948.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40955.0</c:v>
+                  <c:v>40934</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40955</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40962</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$F$15</c:f>
+              <c:f>Sheet1!$B$15:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1041,53 +980,58 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$F$13</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>40927.0</c:v>
+              <c:f>Sheet1!$B$13:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>40927</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40941.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40948.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40955.0</c:v>
+                  <c:v>40934</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40955</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40962</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$16:$F$16</c:f>
+              <c:f>Sheet1!$B$16:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1108,99 +1052,90 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$F$13</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>40927.0</c:v>
+              <c:f>Sheet1!$B$13:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>40927</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40941.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40948.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40955.0</c:v>
+                  <c:v>40934</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40948</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40955</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40962</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$F$17</c:f>
+              <c:f>Sheet1!$B$17:$G$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="442646568"/>
-        <c:axId val="442649752"/>
+        <c:axId val="92843392"/>
+        <c:axId val="92857472"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="442646568"/>
+        <c:axId val="92843392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="442649752"/>
+        <c:crossAx val="92857472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
-        <c:majorUnit val="7.0"/>
+        <c:majorUnit val="7"/>
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="442649752"/>
+        <c:axId val="92857472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="442646568"/>
+        <c:crossAx val="92843392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1211,21 +1146,19 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.69662962962963"/>
-          <c:y val="0.0611463741704776"/>
-          <c:w val="0.281148148148148"/>
-          <c:h val="0.868984630196335"/>
+          <c:x val="0.69662962962963015"/>
+          <c:y val="6.1146374170477601E-2"/>
+          <c:w val="0.28114814814814798"/>
+          <c:h val="0.86898463019633509"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1640,20 +1573,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="B1" s="1">
         <v>40927</v>
       </c>
@@ -1669,8 +1603,11 @@
       <c r="F1" s="1">
         <v>40955</v>
       </c>
+      <c r="G1" s="1">
+        <v>40962</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1689,8 +1626,11 @@
       <c r="F2">
         <v>5</v>
       </c>
+      <c r="G2">
+        <v>116</v>
+      </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1709,8 +1649,11 @@
       <c r="F3">
         <v>0</v>
       </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1729,8 +1672,11 @@
       <c r="F4">
         <v>47</v>
       </c>
+      <c r="G4">
+        <v>47</v>
+      </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1749,8 +1695,11 @@
       <c r="F5">
         <v>101</v>
       </c>
+      <c r="G5">
+        <v>107</v>
+      </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="B7" s="1">
         <v>40927</v>
       </c>
@@ -1766,8 +1715,11 @@
       <c r="F7" s="1">
         <v>40955</v>
       </c>
+      <c r="G7" s="1">
+        <v>40962</v>
+      </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1781,7 +1733,7 @@
         <v>9574</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1795,7 +1747,7 @@
         <v>7025</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1815,7 +1767,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:7">
       <c r="B13" s="1">
         <v>40927</v>
       </c>
@@ -1831,8 +1783,11 @@
       <c r="F13" s="1">
         <v>40955</v>
       </c>
+      <c r="G13" s="1">
+        <v>40962</v>
+      </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1851,8 +1806,11 @@
       <c r="F14">
         <v>3</v>
       </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1871,8 +1829,11 @@
       <c r="F15">
         <v>1</v>
       </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1891,8 +1852,11 @@
       <c r="F16">
         <v>1</v>
       </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1909,6 +1873,9 @@
         <v>1</v>
       </c>
       <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
         <v>1</v>
       </c>
     </row>
@@ -1925,12 +1892,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1942,12 +1909,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Updated today's briefing and metrics spreadsheet after making edits while at work.
</commit_message>
<xml_diff>
--- a/doc/metrics.xlsx
+++ b/doc/metrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="11985" yWindow="2100" windowWidth="24405" windowHeight="17595"/>
+    <workbookView xWindow="11985" yWindow="2100" windowWidth="24405" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -347,7 +347,7 @@
                   <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>47</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -425,20 +425,19 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="92125824"/>
-        <c:axId val="91427200"/>
+        <c:axId val="120233984"/>
+        <c:axId val="120235520"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="92125824"/>
+        <c:axId val="120233984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91427200"/>
+        <c:crossAx val="120235520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -447,7 +446,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="91427200"/>
+        <c:axId val="120235520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -455,7 +454,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92125824"/>
+        <c:crossAx val="120233984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -466,10 +465,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.66823091247672317"/>
-          <c:y val="4.3679125262180617E-2"/>
-          <c:w val="0.30569832402234604"/>
-          <c:h val="0.90681933317287311"/>
+          <c:x val="0.66823091247672339"/>
+          <c:y val="4.3679125262180603E-2"/>
+          <c:w val="0.30569832402234609"/>
+          <c:h val="0.90681933317287322"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -478,7 +477,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -551,6 +550,9 @@
                 <c:pt idx="4">
                   <c:v>9574</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>9574</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -614,17 +616,19 @@
                 <c:pt idx="4">
                   <c:v>7025</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>7025</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="91449600"/>
-        <c:axId val="91467776"/>
+        <c:axId val="123022720"/>
+        <c:axId val="123024512"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="91449600"/>
+        <c:axId val="123022720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -641,7 +645,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91467776"/>
+        <c:crossAx val="123024512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -650,7 +654,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="91467776"/>
+        <c:axId val="123024512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -658,7 +662,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91449600"/>
+        <c:crossAx val="123022720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -672,7 +676,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -754,24 +758,26 @@
                 <c:pt idx="4">
                   <c:v>107</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>112</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="92805376"/>
-        <c:axId val="92815360"/>
+        <c:axId val="123047296"/>
+        <c:axId val="123049088"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="92805376"/>
+        <c:axId val="123047296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92815360"/>
+        <c:crossAx val="123049088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -780,7 +786,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="92815360"/>
+        <c:axId val="123049088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="80"/>
@@ -789,7 +795,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92805376"/>
+        <c:crossAx val="123047296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -803,7 +809,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -955,7 +961,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1105,20 +1111,19 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="92843392"/>
-        <c:axId val="92857472"/>
+        <c:axId val="123106048"/>
+        <c:axId val="123107584"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="92843392"/>
+        <c:axId val="123106048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92857472"/>
+        <c:crossAx val="123107584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1127,7 +1132,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="92857472"/>
+        <c:axId val="123107584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1135,7 +1140,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92843392"/>
+        <c:crossAx val="123106048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1146,10 +1151,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.69662962962963015"/>
+          <c:x val="0.69662962962963026"/>
           <c:y val="6.1146374170477601E-2"/>
-          <c:w val="0.28114814814814798"/>
-          <c:h val="0.86898463019633509"/>
+          <c:w val="0.28114814814814792"/>
+          <c:h val="0.86898463019633521"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -1158,7 +1163,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1576,8 +1581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1673,7 +1678,7 @@
         <v>47</v>
       </c>
       <c r="G4">
-        <v>47</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1732,6 +1737,9 @@
       <c r="F8">
         <v>9574</v>
       </c>
+      <c r="G8">
+        <v>9574</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
@@ -1746,6 +1754,9 @@
       <c r="F9">
         <v>7025</v>
       </c>
+      <c r="G9">
+        <v>7025</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
@@ -1766,6 +1777,9 @@
       <c r="F11">
         <v>107</v>
       </c>
+      <c r="G11">
+        <v>112</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="B13" s="1">
@@ -1830,7 +1844,7 @@
         <v>1</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:7">

</xml_diff>

<commit_message>
Added status update slides for March 15.
</commit_message>
<xml_diff>
--- a/doc/metrics.xlsx
+++ b/doc/metrics.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="11985" yWindow="2100" windowWidth="24405" windowHeight="13740"/>
+    <workbookView xWindow="11985" yWindow="2100" windowWidth="21720" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,8 +59,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,17 +126,34 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -156,10 +173,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:f>Sheet1!$B$1:$J$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -177,16 +194,25 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>40962</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40969</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40976</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$G$2</c:f>
+              <c:f>Sheet1!$B$2:$J$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -203,11 +229,21 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>116</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -228,10 +264,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:f>Sheet1!$B$1:$J$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -249,16 +285,25 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>40962</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40969</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40976</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$G$3</c:f>
+              <c:f>Sheet1!$B$3:$J$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -275,11 +320,21 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -300,10 +355,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:f>Sheet1!$B$1:$J$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -321,16 +376,25 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>40962</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40969</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40976</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$G$4</c:f>
+              <c:f>Sheet1!$B$4:$J$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>47</c:v>
                 </c:pt>
@@ -347,11 +411,21 @@
                   <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>158</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -372,10 +446,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:f>Sheet1!$B$1:$J$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -393,16 +467,25 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>40962</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40969</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40976</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$G$5</c:f>
+              <c:f>Sheet1!$B$5:$J$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>70</c:v>
                 </c:pt>
@@ -420,24 +503,46 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>120</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="120233984"/>
-        <c:axId val="120235520"/>
+        <c:smooth val="0"/>
+        <c:axId val="130369408"/>
+        <c:axId val="130370944"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="120233984"/>
+        <c:axId val="130369408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120235520"/>
+        <c:crossAx val="130370944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -446,15 +551,18 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="120235520"/>
+        <c:axId val="130370944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120233984"/>
+        <c:crossAx val="130369408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -471,9 +579,11 @@
           <c:h val="0.90681933317287322"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -485,12 +595,24 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -510,10 +632,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$G$7</c:f>
+              <c:f>Sheet1!$B$7:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -531,16 +653,25 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>40962</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40969</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40976</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$G$8</c:f>
+              <c:f>Sheet1!$B$8:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="2">
                   <c:v>8825</c:v>
                 </c:pt>
@@ -552,10 +683,20 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>9574</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9574</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9574</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9284</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -576,10 +717,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$G$7</c:f>
+              <c:f>Sheet1!$B$7:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -597,16 +738,25 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>40962</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40969</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40976</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$G$9</c:f>
+              <c:f>Sheet1!$B$9:$J$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="2">
                   <c:v>6499</c:v>
                 </c:pt>
@@ -618,22 +768,44 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>7025</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7025</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7025</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7143</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="123022720"/>
-        <c:axId val="123024512"/>
+        <c:smooth val="0"/>
+        <c:axId val="130089344"/>
+        <c:axId val="130090880"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="123022720"/>
+        <c:axId val="130089344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr rot="-2700000"/>
@@ -645,7 +817,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="123024512"/>
+        <c:crossAx val="130090880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -654,15 +826,18 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="123024512"/>
+        <c:axId val="130090880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123022720"/>
+        <c:crossAx val="130089344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -670,9 +845,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -684,15 +861,28 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -712,10 +902,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$G$7</c:f>
+              <c:f>Sheet1!$B$7:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -733,16 +923,25 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>40962</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40969</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40976</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$G$11</c:f>
+              <c:f>Sheet1!$B$11:$J$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>85</c:v>
                 </c:pt>
@@ -759,25 +958,47 @@
                   <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>112</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="123047296"/>
-        <c:axId val="123049088"/>
+        <c:smooth val="0"/>
+        <c:axId val="130110976"/>
+        <c:axId val="130112512"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="123047296"/>
+        <c:axId val="130110976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123049088"/>
+        <c:crossAx val="130112512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -786,16 +1007,19 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="123049088"/>
+        <c:axId val="130112512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="80"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123047296"/>
+        <c:crossAx val="130110976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -803,9 +1027,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -817,12 +1043,24 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -842,10 +1080,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$G$13</c:f>
+              <c:f>Sheet1!$B$13:$J$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -863,16 +1101,25 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>40962</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40969</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40976</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$G$14</c:f>
+              <c:f>Sheet1!$B$14:$J$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -889,11 +1136,21 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -914,10 +1171,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$G$13</c:f>
+              <c:f>Sheet1!$B$13:$J$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -935,16 +1192,25 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>40962</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40969</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40976</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$G$15</c:f>
+              <c:f>Sheet1!$B$15:$J$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -961,11 +1227,21 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -986,10 +1262,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$G$13</c:f>
+              <c:f>Sheet1!$B$13:$J$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -1007,16 +1283,25 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>40962</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40969</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40976</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$16:$G$16</c:f>
+              <c:f>Sheet1!$B$16:$J$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1033,11 +1318,21 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1058,10 +1353,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$G$13</c:f>
+              <c:f>Sheet1!$B$13:$J$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -1079,16 +1374,25 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>40962</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40969</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40976</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$G$17</c:f>
+              <c:f>Sheet1!$B$17:$J$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1106,24 +1410,46 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="123106048"/>
-        <c:axId val="123107584"/>
+        <c:smooth val="0"/>
+        <c:axId val="130147840"/>
+        <c:axId val="130149376"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="123106048"/>
+        <c:axId val="130147840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123107584"/>
+        <c:crossAx val="130149376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1132,15 +1458,18 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="123107584"/>
+        <c:axId val="130149376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123106048"/>
+        <c:crossAx val="130147840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1157,9 +1486,11 @@
           <c:h val="0.86898463019633521"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1203,13 +1534,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -1233,13 +1564,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
@@ -1369,6 +1700,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1403,6 +1735,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1578,21 +1911,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>40927</v>
       </c>
@@ -1611,8 +1946,17 @@
       <c r="G1" s="1">
         <v>40962</v>
       </c>
+      <c r="H1" s="1">
+        <v>40969</v>
+      </c>
+      <c r="I1" s="1">
+        <v>40976</v>
+      </c>
+      <c r="J1" s="1">
+        <v>40983</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1634,8 +1978,17 @@
       <c r="G2">
         <v>116</v>
       </c>
+      <c r="H2">
+        <v>116</v>
+      </c>
+      <c r="I2">
+        <v>116</v>
+      </c>
+      <c r="J2">
+        <v>116</v>
+      </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1657,8 +2010,17 @@
       <c r="G3">
         <v>0</v>
       </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1680,8 +2042,17 @@
       <c r="G4">
         <v>158</v>
       </c>
+      <c r="H4">
+        <v>158</v>
+      </c>
+      <c r="I4">
+        <v>158</v>
+      </c>
+      <c r="J4">
+        <v>158</v>
+      </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1703,8 +2074,17 @@
       <c r="G5">
         <v>107</v>
       </c>
+      <c r="H5">
+        <v>114</v>
+      </c>
+      <c r="I5">
+        <v>114</v>
+      </c>
+      <c r="J5">
+        <v>120</v>
+      </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>40927</v>
       </c>
@@ -1723,8 +2103,17 @@
       <c r="G7" s="1">
         <v>40962</v>
       </c>
+      <c r="H7" s="1">
+        <v>40969</v>
+      </c>
+      <c r="I7" s="1">
+        <v>40976</v>
+      </c>
+      <c r="J7" s="1">
+        <v>40983</v>
+      </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1740,8 +2129,17 @@
       <c r="G8">
         <v>9574</v>
       </c>
+      <c r="H8">
+        <v>9574</v>
+      </c>
+      <c r="I8">
+        <v>9574</v>
+      </c>
+      <c r="J8">
+        <v>9284</v>
+      </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1757,8 +2155,17 @@
       <c r="G9">
         <v>7025</v>
       </c>
+      <c r="H9">
+        <v>7025</v>
+      </c>
+      <c r="I9">
+        <v>7025</v>
+      </c>
+      <c r="J9">
+        <v>7143</v>
+      </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1780,8 +2187,17 @@
       <c r="G11">
         <v>112</v>
       </c>
+      <c r="H11">
+        <v>112</v>
+      </c>
+      <c r="I11">
+        <v>112</v>
+      </c>
+      <c r="J11">
+        <v>112</v>
+      </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>40927</v>
       </c>
@@ -1800,8 +2216,17 @@
       <c r="G13" s="1">
         <v>40962</v>
       </c>
+      <c r="H13" s="1">
+        <v>40969</v>
+      </c>
+      <c r="I13" s="1">
+        <v>40976</v>
+      </c>
+      <c r="J13" s="1">
+        <v>40983</v>
+      </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1823,8 +2248,17 @@
       <c r="G14">
         <v>3</v>
       </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <v>3</v>
+      </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1846,8 +2280,17 @@
       <c r="G15">
         <v>2</v>
       </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1869,8 +2312,17 @@
       <c r="G16">
         <v>1</v>
       </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1891,6 +2343,15 @@
       </c>
       <c r="G17">
         <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1906,12 +2367,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1923,12 +2384,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Corrected file count in metrics spreadsheet and status slides.
</commit_message>
<xml_diff>
--- a/doc/metrics.xlsx
+++ b/doc/metrics.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="11985" yWindow="2100" windowWidth="21720" windowHeight="13620"/>
@@ -59,8 +59,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,24 +136,12 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -243,7 +231,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -334,7 +321,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -425,7 +411,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -516,33 +501,21 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="130369408"/>
-        <c:axId val="130370944"/>
+        <c:axId val="103368960"/>
+        <c:axId val="103391232"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="130369408"/>
+        <c:axId val="103368960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130370944"/>
+        <c:crossAx val="103391232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -551,18 +524,15 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="130370944"/>
+        <c:axId val="103391232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130369408"/>
+        <c:crossAx val="103368960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -573,21 +543,19 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.66823091247672339"/>
-          <c:y val="4.3679125262180603E-2"/>
-          <c:w val="0.30569832402234609"/>
-          <c:h val="0.90681933317287322"/>
+          <c:x val="0.66823091247672362"/>
+          <c:y val="4.3679125262180582E-2"/>
+          <c:w val="0.30569832402234615"/>
+          <c:h val="0.90681933317287333"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -595,24 +563,12 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -696,7 +652,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -781,31 +736,19 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="130089344"/>
-        <c:axId val="130090880"/>
+        <c:axId val="138368896"/>
+        <c:axId val="138370432"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="130089344"/>
+        <c:axId val="138368896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr rot="-2700000"/>
@@ -817,7 +760,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="130090880"/>
+        <c:crossAx val="138370432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -826,18 +769,15 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="130090880"/>
+        <c:axId val="138370432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130089344"/>
+        <c:crossAx val="138368896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -845,15 +785,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -861,28 +799,15 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -967,38 +892,26 @@
                   <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>112</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="130110976"/>
-        <c:axId val="130112512"/>
+        <c:axId val="138282880"/>
+        <c:axId val="138284416"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="130110976"/>
+        <c:axId val="138282880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130112512"/>
+        <c:crossAx val="138284416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1007,19 +920,16 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="130112512"/>
+        <c:axId val="138284416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="80"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130110976"/>
+        <c:crossAx val="138282880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1027,15 +937,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1043,24 +951,12 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1150,7 +1046,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1241,7 +1136,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1332,7 +1226,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1423,33 +1316,21 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="130147840"/>
-        <c:axId val="130149376"/>
+        <c:axId val="138320896"/>
+        <c:axId val="138334976"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="130147840"/>
+        <c:axId val="138320896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130149376"/>
+        <c:crossAx val="138334976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1458,18 +1339,15 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="130149376"/>
+        <c:axId val="138334976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130147840"/>
+        <c:crossAx val="138320896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1480,21 +1358,19 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.69662962962963026"/>
+          <c:x val="0.69662962962963049"/>
           <c:y val="6.1146374170477601E-2"/>
-          <c:w val="0.28114814814814792"/>
-          <c:h val="0.86898463019633521"/>
+          <c:w val="0.28114814814814787"/>
+          <c:h val="0.86898463019633532"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1700,7 +1576,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1735,7 +1610,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1911,14 +1785,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -1927,7 +1801,7 @@
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="B1" s="1">
         <v>40927</v>
       </c>
@@ -1956,7 +1830,7 @@
         <v>40983</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1988,7 +1862,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2020,7 +1894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2052,7 +1926,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2084,7 +1958,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="B7" s="1">
         <v>40927</v>
       </c>
@@ -2113,7 +1987,7 @@
         <v>40983</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2139,7 +2013,7 @@
         <v>9284</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2165,7 +2039,7 @@
         <v>7143</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -2194,10 +2068,10 @@
         <v>112</v>
       </c>
       <c r="J11">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="B13" s="1">
         <v>40927</v>
       </c>
@@ -2226,7 +2100,7 @@
         <v>40983</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -2258,7 +2132,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -2290,7 +2164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -2322,7 +2196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -2367,12 +2241,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2384,12 +2258,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Updated metrics, added status brief and temp sensor pics
</commit_message>
<xml_diff>
--- a/doc/metrics.xlsx
+++ b/doc/metrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="11985" yWindow="2100" windowWidth="21720" windowHeight="13620"/>
+    <workbookView xWindow="11985" yWindow="2100" windowWidth="19440" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -161,10 +161,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$J$1</c:f>
+              <c:f>Sheet1!$B$1:$K$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -191,16 +191,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>40983</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$J$2</c:f>
+              <c:f>Sheet1!$B$2:$K$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -226,6 +229,9 @@
                   <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>116</c:v>
                 </c:pt>
               </c:numCache>
@@ -251,10 +257,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$J$1</c:f>
+              <c:f>Sheet1!$B$1:$K$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -281,16 +287,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>40983</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$J$3</c:f>
+              <c:f>Sheet1!$B$3:$K$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -316,6 +325,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -341,10 +353,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$J$1</c:f>
+              <c:f>Sheet1!$B$1:$K$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -371,16 +383,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>40983</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$J$4</c:f>
+              <c:f>Sheet1!$B$4:$K$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>47</c:v>
                 </c:pt>
@@ -406,6 +421,9 @@
                   <c:v>158</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>158</c:v>
                 </c:pt>
               </c:numCache>
@@ -431,10 +449,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$J$1</c:f>
+              <c:f>Sheet1!$B$1:$K$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -461,16 +479,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>40983</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$J$5</c:f>
+              <c:f>Sheet1!$B$5:$K$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>70</c:v>
                 </c:pt>
@@ -497,25 +518,27 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>127</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="103368960"/>
-        <c:axId val="103391232"/>
+        <c:axId val="95926912"/>
+        <c:axId val="96088448"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="103368960"/>
+        <c:axId val="95926912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103391232"/>
+        <c:crossAx val="96088448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -524,7 +547,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="103391232"/>
+        <c:axId val="96088448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -532,7 +555,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103368960"/>
+        <c:crossAx val="95926912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -543,10 +566,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.66823091247672362"/>
-          <c:y val="4.3679125262180582E-2"/>
-          <c:w val="0.30569832402234615"/>
-          <c:h val="0.90681933317287333"/>
+          <c:x val="0.66823091247672373"/>
+          <c:y val="4.3679125262180561E-2"/>
+          <c:w val="0.3056983240223462"/>
+          <c:h val="0.90681933317287344"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -555,7 +578,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -588,10 +611,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$J$7</c:f>
+              <c:f>Sheet1!$B$7:$K$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -618,16 +641,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>40983</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$J$8</c:f>
+              <c:f>Sheet1!$B$8:$K$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="2">
                   <c:v>8825</c:v>
                 </c:pt>
@@ -648,6 +674,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>9284</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9203</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -672,10 +701,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$J$7</c:f>
+              <c:f>Sheet1!$B$7:$K$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -702,16 +731,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>40983</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$J$9</c:f>
+              <c:f>Sheet1!$B$9:$K$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="2">
                   <c:v>6499</c:v>
                 </c:pt>
@@ -732,18 +764,20 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>7143</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8073</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="138368896"/>
-        <c:axId val="138370432"/>
+        <c:axId val="96484352"/>
+        <c:axId val="96560256"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="138368896"/>
+        <c:axId val="96484352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -760,7 +794,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="138370432"/>
+        <c:crossAx val="96560256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -769,7 +803,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="138370432"/>
+        <c:axId val="96560256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -777,7 +811,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138368896"/>
+        <c:crossAx val="96484352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -791,7 +825,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -827,10 +861,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$J$7</c:f>
+              <c:f>Sheet1!$B$7:$K$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -857,16 +891,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>40983</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$J$11</c:f>
+              <c:f>Sheet1!$B$11:$K$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>85</c:v>
                 </c:pt>
@@ -893,25 +930,27 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>114</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="138282880"/>
-        <c:axId val="138284416"/>
+        <c:axId val="39508608"/>
+        <c:axId val="39514496"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="138282880"/>
+        <c:axId val="39508608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138284416"/>
+        <c:crossAx val="39514496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -920,7 +959,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="138284416"/>
+        <c:axId val="39514496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="80"/>
@@ -929,7 +968,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138282880"/>
+        <c:crossAx val="39508608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -943,7 +982,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -976,10 +1015,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$J$13</c:f>
+              <c:f>Sheet1!$B$13:$K$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -1006,16 +1045,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>40983</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$J$14</c:f>
+              <c:f>Sheet1!$B$14:$K$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -1041,6 +1083,9 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
@@ -1066,10 +1111,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$J$13</c:f>
+              <c:f>Sheet1!$B$13:$K$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -1096,16 +1141,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>40983</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$J$15</c:f>
+              <c:f>Sheet1!$B$15:$K$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1131,6 +1179,9 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
@@ -1156,10 +1207,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$J$13</c:f>
+              <c:f>Sheet1!$B$13:$K$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -1186,16 +1237,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>40983</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$16:$J$16</c:f>
+              <c:f>Sheet1!$B$16:$K$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1222,6 +1276,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1246,10 +1303,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$J$13</c:f>
+              <c:f>Sheet1!$B$13:$K$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>40927</c:v>
                 </c:pt>
@@ -1276,16 +1333,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>40983</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$J$17</c:f>
+              <c:f>Sheet1!$B$17:$K$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1311,26 +1371,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="138320896"/>
-        <c:axId val="138334976"/>
+        <c:axId val="39550976"/>
+        <c:axId val="39552512"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="138320896"/>
+        <c:axId val="39550976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138334976"/>
+        <c:crossAx val="39552512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1339,7 +1401,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="138334976"/>
+        <c:axId val="39552512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1347,7 +1409,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138320896"/>
+        <c:crossAx val="39550976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1358,10 +1420,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.69662962962963049"/>
+          <c:x val="0.69662962962963071"/>
           <c:y val="6.1146374170477601E-2"/>
-          <c:w val="0.28114814814814787"/>
-          <c:h val="0.86898463019633532"/>
+          <c:w val="0.28114814814814781"/>
+          <c:h val="0.86898463019633543"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -1370,7 +1432,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1410,16 +1472,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1441,15 +1503,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1786,10 +1848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1798,10 +1860,10 @@
     <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="9.7109375" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="B1" s="1">
         <v>40927</v>
       </c>
@@ -1829,8 +1891,11 @@
       <c r="J1" s="1">
         <v>40983</v>
       </c>
+      <c r="K1" s="1">
+        <v>40997</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1861,8 +1926,11 @@
       <c r="J2">
         <v>116</v>
       </c>
+      <c r="K2">
+        <v>116</v>
+      </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1893,8 +1961,11 @@
       <c r="J3">
         <v>0</v>
       </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1925,8 +1996,11 @@
       <c r="J4">
         <v>158</v>
       </c>
+      <c r="K4">
+        <v>158</v>
+      </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1957,8 +2031,11 @@
       <c r="J5">
         <v>120</v>
       </c>
+      <c r="K5">
+        <v>127</v>
+      </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="B7" s="1">
         <v>40927</v>
       </c>
@@ -1986,8 +2063,11 @@
       <c r="J7" s="1">
         <v>40983</v>
       </c>
+      <c r="K7" s="1">
+        <v>40997</v>
+      </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2012,8 +2092,11 @@
       <c r="J8">
         <v>9284</v>
       </c>
+      <c r="K8">
+        <v>9203</v>
+      </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2038,8 +2121,11 @@
       <c r="J9">
         <v>7143</v>
       </c>
+      <c r="K9">
+        <v>8073</v>
+      </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -2070,8 +2156,11 @@
       <c r="J11">
         <v>116</v>
       </c>
+      <c r="K11">
+        <v>114</v>
+      </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="B13" s="1">
         <v>40927</v>
       </c>
@@ -2099,8 +2188,11 @@
       <c r="J13" s="1">
         <v>40983</v>
       </c>
+      <c r="K13" s="1">
+        <v>40997</v>
+      </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -2131,8 +2223,11 @@
       <c r="J14">
         <v>3</v>
       </c>
+      <c r="K14">
+        <v>3</v>
+      </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -2163,8 +2258,11 @@
       <c r="J15">
         <v>2</v>
       </c>
+      <c r="K15">
+        <v>2</v>
+      </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -2195,8 +2293,11 @@
       <c r="J16">
         <v>1</v>
       </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -2225,13 +2326,16 @@
         <v>1</v>
       </c>
       <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="K17">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Completed status for this wk -- issues with our sloc counter.
</commit_message>
<xml_diff>
--- a/doc/metrics.xlsx
+++ b/doc/metrics.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11985" yWindow="2100" windowWidth="19440" windowHeight="13620"/>
+    <workbookView xWindow="7240" yWindow="180" windowWidth="31100" windowHeight="20760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,8 +59,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,8 +102,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -115,13 +121,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -136,12 +148,24 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -161,82 +185,95 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$K$1</c:f>
+              <c:f>Sheet1!$B$1:$M$1</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>40927</c:v>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>40927.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934</c:v>
+                  <c:v>40934.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40941</c:v>
+                  <c:v>40941.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40948</c:v>
+                  <c:v>40948.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40955</c:v>
+                  <c:v>40955.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40962</c:v>
+                  <c:v>40962.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40969</c:v>
+                  <c:v>40969.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40976</c:v>
+                  <c:v>40976.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40983</c:v>
+                  <c:v>40983.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40997</c:v>
+                  <c:v>40997.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41004.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41011.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$K$2</c:f>
+              <c:f>Sheet1!$B$2:$M$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>116</c:v>
+                  <c:v>116.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>116</c:v>
+                  <c:v>116.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>116</c:v>
+                  <c:v>116.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>116</c:v>
+                  <c:v>116.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>116</c:v>
+                  <c:v>116.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>116.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>116.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -257,82 +294,95 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$K$1</c:f>
+              <c:f>Sheet1!$B$1:$M$1</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>40927</c:v>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>40927.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934</c:v>
+                  <c:v>40934.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40941</c:v>
+                  <c:v>40941.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40948</c:v>
+                  <c:v>40948.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40955</c:v>
+                  <c:v>40955.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40962</c:v>
+                  <c:v>40962.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40969</c:v>
+                  <c:v>40969.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40976</c:v>
+                  <c:v>40976.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40983</c:v>
+                  <c:v>40983.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40997</c:v>
+                  <c:v>40997.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41004.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41011.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$K$3</c:f>
+              <c:f>Sheet1!$B$3:$M$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -353,82 +403,95 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$K$1</c:f>
+              <c:f>Sheet1!$B$1:$M$1</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>40927</c:v>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>40927.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934</c:v>
+                  <c:v>40934.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40941</c:v>
+                  <c:v>40941.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40948</c:v>
+                  <c:v>40948.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40955</c:v>
+                  <c:v>40955.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40962</c:v>
+                  <c:v>40962.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40969</c:v>
+                  <c:v>40969.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40976</c:v>
+                  <c:v>40976.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40983</c:v>
+                  <c:v>40983.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40997</c:v>
+                  <c:v>40997.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41004.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41011.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$K$4</c:f>
+              <c:f>Sheet1!$B$4:$M$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>47</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>47.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>47</c:v>
+                  <c:v>47.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>47</c:v>
+                  <c:v>47.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>47</c:v>
+                  <c:v>47.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>47</c:v>
+                  <c:v>47.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>158</c:v>
+                  <c:v>158.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>158</c:v>
+                  <c:v>158.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>158</c:v>
+                  <c:v>158.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>158</c:v>
+                  <c:v>158.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>158</c:v>
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>158.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -449,113 +512,141 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$K$1</c:f>
+              <c:f>Sheet1!$B$1:$M$1</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>40927</c:v>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>40927.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934</c:v>
+                  <c:v>40934.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40941</c:v>
+                  <c:v>40941.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40948</c:v>
+                  <c:v>40948.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40955</c:v>
+                  <c:v>40955.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40962</c:v>
+                  <c:v>40962.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40969</c:v>
+                  <c:v>40969.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40976</c:v>
+                  <c:v>40976.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40983</c:v>
+                  <c:v>40983.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40997</c:v>
+                  <c:v>40997.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41004.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41011.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$K$5</c:f>
+              <c:f>Sheet1!$B$5:$M$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>70</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>70.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>76</c:v>
+                  <c:v>76.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>84</c:v>
+                  <c:v>84.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>93</c:v>
+                  <c:v>93.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>101</c:v>
+                  <c:v>101.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>107</c:v>
+                  <c:v>107.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>114</c:v>
+                  <c:v>114.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>114</c:v>
+                  <c:v>114.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>120</c:v>
+                  <c:v>120.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>127</c:v>
+                  <c:v>127.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>134.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>149.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="95926912"/>
-        <c:axId val="96088448"/>
+        <c:smooth val="0"/>
+        <c:axId val="424389416"/>
+        <c:axId val="424392600"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="95926912"/>
+        <c:axId val="424389416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96088448"/>
+        <c:crossAx val="424392600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
-        <c:majorUnit val="7"/>
+        <c:majorUnit val="7.0"/>
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="96088448"/>
+        <c:axId val="424392600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95926912"/>
+        <c:crossAx val="424389416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -566,19 +657,21 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.66823091247672373"/>
-          <c:y val="4.3679125262180561E-2"/>
-          <c:w val="0.3056983240223462"/>
-          <c:h val="0.90681933317287344"/>
+          <c:x val="0.668230912476724"/>
+          <c:y val="0.0436791252621805"/>
+          <c:w val="0.305698324022346"/>
+          <c:h val="0.906819333172874"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -586,12 +679,24 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -611,76 +716,89 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$K$7</c:f>
+              <c:f>Sheet1!$B$7:$M$7</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>40927</c:v>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>40927.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934</c:v>
+                  <c:v>40934.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40941</c:v>
+                  <c:v>40941.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40948</c:v>
+                  <c:v>40948.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40955</c:v>
+                  <c:v>40955.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40962</c:v>
+                  <c:v>40962.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40969</c:v>
+                  <c:v>40969.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40976</c:v>
+                  <c:v>40976.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40983</c:v>
+                  <c:v>40983.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40997</c:v>
+                  <c:v>40997.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41004.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41011.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$K$8</c:f>
+              <c:f>Sheet1!$B$8:$M$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="2">
-                  <c:v>8825</c:v>
+                  <c:v>8825.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9092</c:v>
+                  <c:v>9092.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9574</c:v>
+                  <c:v>9574.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9574</c:v>
+                  <c:v>9574.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9574</c:v>
+                  <c:v>9574.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9574</c:v>
+                  <c:v>9574.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9284</c:v>
+                  <c:v>9284.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9203</c:v>
+                  <c:v>9203.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9325.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9325.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -701,88 +819,113 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$K$7</c:f>
+              <c:f>Sheet1!$B$7:$M$7</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>40927</c:v>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>40927.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934</c:v>
+                  <c:v>40934.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40941</c:v>
+                  <c:v>40941.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40948</c:v>
+                  <c:v>40948.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40955</c:v>
+                  <c:v>40955.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40962</c:v>
+                  <c:v>40962.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40969</c:v>
+                  <c:v>40969.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40976</c:v>
+                  <c:v>40976.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40983</c:v>
+                  <c:v>40983.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40997</c:v>
+                  <c:v>40997.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41004.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41011.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$K$9</c:f>
+              <c:f>Sheet1!$B$9:$M$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="2">
-                  <c:v>6499</c:v>
+                  <c:v>6499.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6693</c:v>
+                  <c:v>6693.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7025</c:v>
+                  <c:v>7025.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7025</c:v>
+                  <c:v>7025.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7025</c:v>
+                  <c:v>7025.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7025</c:v>
+                  <c:v>7025.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7143</c:v>
+                  <c:v>7143.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8073</c:v>
+                  <c:v>8073.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8158.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8158.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="96484352"/>
-        <c:axId val="96560256"/>
+        <c:smooth val="0"/>
+        <c:axId val="424451112"/>
+        <c:axId val="424454184"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="96484352"/>
+        <c:axId val="424451112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr rot="-2700000"/>
@@ -794,24 +937,28 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96560256"/>
+        <c:crossAx val="424454184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
-        <c:majorUnit val="7"/>
+        <c:majorUnit val="7.0"/>
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="96560256"/>
+        <c:axId val="424454184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="6000.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96484352"/>
+        <c:crossAx val="424451112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -819,13 +966,15 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -833,15 +982,28 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -861,114 +1023,142 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$K$7</c:f>
+              <c:f>Sheet1!$B$7:$M$7</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>40927</c:v>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>40927.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934</c:v>
+                  <c:v>40934.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40941</c:v>
+                  <c:v>40941.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40948</c:v>
+                  <c:v>40948.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40955</c:v>
+                  <c:v>40955.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40962</c:v>
+                  <c:v>40962.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40969</c:v>
+                  <c:v>40969.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40976</c:v>
+                  <c:v>40976.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40983</c:v>
+                  <c:v>40983.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40997</c:v>
+                  <c:v>40997.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41004.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41011.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$K$11</c:f>
+              <c:f>Sheet1!$B$11:$M$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>85</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>85.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85</c:v>
+                  <c:v>85.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>96</c:v>
+                  <c:v>96.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>97</c:v>
+                  <c:v>97.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>107</c:v>
+                  <c:v>107.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>112</c:v>
+                  <c:v>112.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>112</c:v>
+                  <c:v>112.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>112</c:v>
+                  <c:v>112.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>116</c:v>
+                  <c:v>116.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>114</c:v>
+                  <c:v>114.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>114.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>131.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="39508608"/>
-        <c:axId val="39514496"/>
+        <c:smooth val="0"/>
+        <c:axId val="424476104"/>
+        <c:axId val="424479128"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="39508608"/>
+        <c:axId val="424476104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39514496"/>
+        <c:crossAx val="424479128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
-        <c:majorUnit val="7"/>
+        <c:majorUnit val="7.0"/>
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="39514496"/>
+        <c:axId val="424479128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="80"/>
+          <c:min val="80.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39508608"/>
+        <c:crossAx val="424476104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -976,13 +1166,15 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -990,12 +1182,24 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1015,82 +1219,95 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$K$13</c:f>
+              <c:f>Sheet1!$B$13:$M$13</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>40927</c:v>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>40927.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934</c:v>
+                  <c:v>40934.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40941</c:v>
+                  <c:v>40941.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40948</c:v>
+                  <c:v>40948.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40955</c:v>
+                  <c:v>40955.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40962</c:v>
+                  <c:v>40962.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40969</c:v>
+                  <c:v>40969.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40976</c:v>
+                  <c:v>40976.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40983</c:v>
+                  <c:v>40983.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40997</c:v>
+                  <c:v>40997.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41004.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41011.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$K$14</c:f>
+              <c:f>Sheet1!$B$14:$M$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1111,82 +1328,95 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$K$13</c:f>
+              <c:f>Sheet1!$B$13:$M$13</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>40927</c:v>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>40927.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934</c:v>
+                  <c:v>40934.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40941</c:v>
+                  <c:v>40941.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40948</c:v>
+                  <c:v>40948.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40955</c:v>
+                  <c:v>40955.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40962</c:v>
+                  <c:v>40962.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40969</c:v>
+                  <c:v>40969.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40976</c:v>
+                  <c:v>40976.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40983</c:v>
+                  <c:v>40983.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40997</c:v>
+                  <c:v>40997.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41004.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41011.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$K$15</c:f>
+              <c:f>Sheet1!$B$15:$M$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1207,82 +1437,95 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$K$13</c:f>
+              <c:f>Sheet1!$B$13:$M$13</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>40927</c:v>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>40927.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934</c:v>
+                  <c:v>40934.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40941</c:v>
+                  <c:v>40941.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40948</c:v>
+                  <c:v>40948.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40955</c:v>
+                  <c:v>40955.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40962</c:v>
+                  <c:v>40962.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40969</c:v>
+                  <c:v>40969.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40976</c:v>
+                  <c:v>40976.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40983</c:v>
+                  <c:v>40983.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40997</c:v>
+                  <c:v>40997.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41004.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41011.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$16:$K$16</c:f>
+              <c:f>Sheet1!$B$16:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1303,113 +1546,141 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$K$13</c:f>
+              <c:f>Sheet1!$B$13:$M$13</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>40927</c:v>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>40927.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40934</c:v>
+                  <c:v>40934.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40941</c:v>
+                  <c:v>40941.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40948</c:v>
+                  <c:v>40948.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40955</c:v>
+                  <c:v>40955.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40962</c:v>
+                  <c:v>40962.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40969</c:v>
+                  <c:v>40969.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40976</c:v>
+                  <c:v>40976.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40983</c:v>
+                  <c:v>40983.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40997</c:v>
+                  <c:v>40997.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41004.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41011.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$K$17</c:f>
+              <c:f>Sheet1!$B$17:$M$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="39550976"/>
-        <c:axId val="39552512"/>
+        <c:smooth val="0"/>
+        <c:axId val="424523640"/>
+        <c:axId val="424526824"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="39550976"/>
+        <c:axId val="424523640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39552512"/>
+        <c:crossAx val="424526824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
-        <c:majorUnit val="7"/>
+        <c:majorUnit val="7.0"/>
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="39552512"/>
+        <c:axId val="424526824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39550976"/>
+        <c:crossAx val="424523640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1420,19 +1691,21 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.69662962962963071"/>
-          <c:y val="6.1146374170477601E-2"/>
-          <c:w val="0.28114814814814781"/>
-          <c:h val="0.86898463019633543"/>
+          <c:x val="0.696629629629631"/>
+          <c:y val="0.0611463741704776"/>
+          <c:w val="0.281148148148148"/>
+          <c:h val="0.868984630196335"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1478,10 +1751,10 @@
       <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1847,23 +2120,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.7109375" customWidth="1"/>
-    <col min="10" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.6640625" customWidth="1"/>
+    <col min="10" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="B1" s="1">
         <v>40927</v>
       </c>
@@ -1894,8 +2167,14 @@
       <c r="K1" s="1">
         <v>40997</v>
       </c>
+      <c r="L1" s="1">
+        <v>41004</v>
+      </c>
+      <c r="M1" s="1">
+        <v>41011</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1929,8 +2208,14 @@
       <c r="K2">
         <v>116</v>
       </c>
+      <c r="L2">
+        <v>116</v>
+      </c>
+      <c r="M2">
+        <v>116</v>
+      </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1964,8 +2249,14 @@
       <c r="K3">
         <v>0</v>
       </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1999,8 +2290,14 @@
       <c r="K4">
         <v>158</v>
       </c>
+      <c r="L4">
+        <v>158</v>
+      </c>
+      <c r="M4">
+        <v>158</v>
+      </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2034,8 +2331,15 @@
       <c r="K5">
         <v>127</v>
       </c>
+      <c r="L5">
+        <v>134</v>
+      </c>
+      <c r="M5">
+        <f>134+15</f>
+        <v>149</v>
+      </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:13">
       <c r="B7" s="1">
         <v>40927</v>
       </c>
@@ -2066,8 +2370,14 @@
       <c r="K7" s="1">
         <v>40997</v>
       </c>
+      <c r="L7" s="1">
+        <v>41004</v>
+      </c>
+      <c r="M7" s="1">
+        <v>41011</v>
+      </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2095,8 +2405,14 @@
       <c r="K8">
         <v>9203</v>
       </c>
+      <c r="L8">
+        <v>9325</v>
+      </c>
+      <c r="M8">
+        <v>9325</v>
+      </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2124,8 +2440,14 @@
       <c r="K9">
         <v>8073</v>
       </c>
+      <c r="L9">
+        <v>8158</v>
+      </c>
+      <c r="M9">
+        <v>8158</v>
+      </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -2159,8 +2481,14 @@
       <c r="K11">
         <v>114</v>
       </c>
+      <c r="L11">
+        <v>114</v>
+      </c>
+      <c r="M11">
+        <v>131</v>
+      </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:13">
       <c r="B13" s="1">
         <v>40927</v>
       </c>
@@ -2191,8 +2519,14 @@
       <c r="K13" s="1">
         <v>40997</v>
       </c>
+      <c r="L13" s="1">
+        <v>41004</v>
+      </c>
+      <c r="M13" s="1">
+        <v>41011</v>
+      </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -2226,8 +2560,14 @@
       <c r="K14">
         <v>3</v>
       </c>
+      <c r="L14">
+        <v>3</v>
+      </c>
+      <c r="M14">
+        <v>3</v>
+      </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -2261,8 +2601,14 @@
       <c r="K15">
         <v>2</v>
       </c>
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -2296,8 +2642,14 @@
       <c r="K16">
         <v>2</v>
       </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="M16">
+        <v>2</v>
+      </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -2329,13 +2681,19 @@
         <v>2</v>
       </c>
       <c r="K17">
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <v>2</v>
+      </c>
+      <c r="M17">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2345,12 +2703,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2362,12 +2720,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>